<commit_message>
Tidied up exceptions and serialisation logic
</commit_message>
<xml_diff>
--- a/FOMS/data/branch_list.xlsx
+++ b/FOMS/data/branch_list.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\Documents\GitHub\SC2002_OOP_FOMS\FOMS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAC9D46-8EB6-42B2-BDC1-2C433BE2E948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62817BB-E123-4364-9AF9-AF2C0DA012C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
   </bookViews>
   <sheets>
-    <sheet name="staff" sheetId="1" r:id="rId1"/>
+    <sheet name="branch" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">staff!$A$1:$A$88</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">staff!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">branch!$A$1:$A$88</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">branch!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +29,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>staffQuota</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>North spine Plaza</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>Jurong point</t>
+  </si>
+  <si>
+    <t>JE</t>
+  </si>
+  <si>
+    <t>Jurong east</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>477c0c7e-9d46-4202-969d-f3dd1933a575</t>
+  </si>
+  <si>
+    <t>67136f7c-fcd0-45f1-8859-9e3d183faeb3</t>
+  </si>
+  <si>
+    <t>5cc0e578-41b6-4e7d-b6e8-5f287be3e857</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,12 +472,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
-  <dimension ref="A1:A87"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,52 +487,96 @@
     <col min="3" max="3" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8"/>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated file structure and fixed transfer staff
</commit_message>
<xml_diff>
--- a/FOMS/data/branch_list.xlsx
+++ b/FOMS/data/branch_list.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -80,6 +80,15 @@
   </si>
   <si>
     <t>20e7adc4-0f30-4019-b1d1-cb2a8d998616</t>
+  </si>
+  <si>
+    <t>cccb4419-e7e1-4f63-b0f2-b9af8c6256c6</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>3da2a086-a730-4d99-9d7e-7ea5af4bf172</t>
   </si>
 </sst>
 </file>
@@ -485,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -563,16 +572,16 @@
       <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+      <c r="A9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
+      <c r="A10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
@@ -583,23 +592,23 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
+      <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
+      <c r="A17" s="1"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
+      <c r="A19" s="3"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
@@ -617,13 +626,13 @@
       <c r="A24" s="3"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3"/>
+      <c r="A25" s="4"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
+      <c r="A27" s="3"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
@@ -650,25 +659,25 @@
       <c r="A35" s="3"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="3"/>
+      <c r="A36" s="1"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="1"/>
+      <c r="A38" s="3"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="3"/>
+      <c r="A40" s="1"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" s="1"/>
+      <c r="A42" s="3"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
@@ -695,25 +704,25 @@
       <c r="A50" s="3"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" s="3"/>
+      <c r="A51" s="7"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" s="3"/>
+      <c r="A52" s="1"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" s="7"/>
+      <c r="A53" s="3"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" s="1"/>
+      <c r="A54" s="3"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" s="3"/>
+      <c r="A55" s="1"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" s="3"/>
+      <c r="A56" s="1"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" s="1"/>
+      <c r="A57" s="3"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
@@ -722,7 +731,7 @@
       <c r="A59" s="3"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60" s="1"/>
+      <c r="A60" s="3"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="3"/>
@@ -739,11 +748,11 @@
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="3"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" s="3"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67" s="3"/>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="2"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="2"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="2"/>
@@ -765,12 +774,6 @@
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="2"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A77" s="2"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A78" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Updated files for code logic
</commit_message>
<xml_diff>
--- a/FOMS/data/branch_list.xlsx
+++ b/FOMS/data/branch_list.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>6b4b325a-a060-46ce-969c-a5a427566f4b</t>
   </si>
 </sst>
 </file>
@@ -597,8 +600,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>

</xml_diff>

<commit_message>
Updated display of order for staff
</commit_message>
<xml_diff>
--- a/FOMS/data/branch_list.xlsx
+++ b/FOMS/data/branch_list.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\Documents\GitHub\SC2002_OOP_FOMS\FOMS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59EA764-7C76-4908-BFA0-EDD912B028BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DD94CB-4C0F-4C88-AAFF-9DE545959923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>name</t>
   </si>
@@ -68,43 +68,12 @@
   </si>
   <si>
     <t>Jurong East</t>
-  </si>
-  <si>
-    <t>AMK</t>
-  </si>
-  <si>
-    <t>Ang Mo Kio</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>20e7adc4-0f30-4019-b1d1-cb2a8d998616</t>
-  </si>
-  <si>
-    <t>cccb4419-e7e1-4f63-b0f2-b9af8c6256c6</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>3da2a086-a730-4d99-9d7e-7ea5af4bf172</t>
-  </si>
-  <si>
-    <t>2e45f62b-ff8d-433b-8a57-c39c49a0d7e5</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>6c37be2e-40bb-439a-a983-a74ee2656acb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -508,14 +477,14 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="5" width="22.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.81640625" collapsed="true"/>
+    <col min="1" max="1" width="22" style="5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.81640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -575,7 +544,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
+      <c r="A5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
@@ -595,19 +564,19 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Edited code to handle NULL values
</commit_message>
<xml_diff>
--- a/FOMS/data/branch_list.xlsx
+++ b/FOMS/data/branch_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\Documents\GitHub\SC2002_OOP_FOMS\FOMS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DD94CB-4C0F-4C88-AAFF-9DE545959923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7C1B9B-713F-4B2B-AD6A-56793B4B4F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t>Jurong East</t>
+  </si>
+  <si>
+    <t>b857ce48-9fe8-42c3-83ee-14ba1287ffc3</t>
+  </si>
+  <si>
+    <t>AMK</t>
+  </si>
+  <si>
+    <t>Ang Mo Kio</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -477,14 +489,15 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22" style="5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.81640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.54296875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -544,7 +557,18 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5"/>
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>

</xml_diff>

<commit_message>
Updated code to handle duplicate branches
</commit_message>
<xml_diff>
--- a/FOMS/data/branch_list.xlsx
+++ b/FOMS/data/branch_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\Documents\GitHub\SC2002_OOP_FOMS\FOMS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7C1B9B-713F-4B2B-AD6A-56793B4B4F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1620EA05-262A-44DF-8269-3892EB02D555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
   </bookViews>
@@ -487,9 +487,9 @@
   <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,7 +571,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
+      <c r="A6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>

</xml_diff>